<commit_message>
Add OSI Svomming cabin trip sign up list
</commit_message>
<xml_diff>
--- a/OSI/2022/01-04-2022 Cabin trip/Sign up order.xlsx
+++ b/OSI/2022/01-04-2022 Cabin trip/Sign up order.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\PhD\OSI\2022\01-04-2022 Cabin trip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC4D9E4-F327-4A09-9FF8-FA15A55B686F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790BE250-5A66-4498-8364-6EA4962DF498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-5085" yWindow="-10890" windowWidth="19380" windowHeight="10980" xr2:uid="{0BDEA556-5F57-4226-85E3-F3754AD378FD}"/>
+    <workbookView xWindow="9450" yWindow="1290" windowWidth="36000" windowHeight="19290" xr2:uid="{0BDEA556-5F57-4226-85E3-F3754AD378FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Håkon</t>
   </si>
@@ -102,13 +102,46 @@
   </si>
   <si>
     <t>Olli Papst</t>
+  </si>
+  <si>
+    <t>Sotiris</t>
+  </si>
+  <si>
+    <t>Synne</t>
+  </si>
+  <si>
+    <t>Feliks</t>
+  </si>
+  <si>
+    <t>Member/Driver</t>
+  </si>
+  <si>
+    <t>Passenger 1</t>
+  </si>
+  <si>
+    <t>Passenger 2</t>
+  </si>
+  <si>
+    <t>Passenger 3</t>
+  </si>
+  <si>
+    <t>Passenger 4</t>
+  </si>
+  <si>
+    <t>Passenger 5</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Elisabeth Greisbauer (facebook name: Elli Sperelli)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,13 +149,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -137,8 +182,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -453,209 +507,331 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB1DDFA6-5E12-4682-95F7-58FCC0495C21}">
-  <dimension ref="A1:B25"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="15" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="11.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3">
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A8">
+      <c r="C8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>19</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19">
+      <c r="B20" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20">
+      <c r="C22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21">
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22">
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B22" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23">
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B23" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>2</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>25</v>
       </c>
     </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add OSI Svomming accounting paperwork
</commit_message>
<xml_diff>
--- a/OSI/2022/01-04-2022 Cabin trip/Sign up order.xlsx
+++ b/OSI/2022/01-04-2022 Cabin trip/Sign up order.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\pc\Dokumenter\PhD\OSI\2022\01-04-2022 Cabin trip\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790BE250-5A66-4498-8364-6EA4962DF498}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6235FF6C-9B72-4619-8373-9F87F7076E04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9450" yWindow="1290" windowWidth="36000" windowHeight="19290" xr2:uid="{0BDEA556-5F57-4226-85E3-F3754AD378FD}"/>
+    <workbookView xWindow="-21588" yWindow="4692" windowWidth="20460" windowHeight="13008" xr2:uid="{0BDEA556-5F57-4226-85E3-F3754AD378FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="38">
   <si>
     <t>Håkon</t>
   </si>
@@ -95,9 +95,6 @@
     <t>Pascaline</t>
   </si>
   <si>
-    <t>Anne Martina</t>
-  </si>
-  <si>
     <t>Tuva</t>
   </si>
   <si>
@@ -135,6 +132,21 @@
   </si>
   <si>
     <t>Elisabeth Greisbauer (facebook name: Elli Sperelli)</t>
+  </si>
+  <si>
+    <t>Manu</t>
+  </si>
+  <si>
+    <t>Hannah</t>
+  </si>
+  <si>
+    <t>Anne Kraus</t>
+  </si>
+  <si>
+    <t>Louis</t>
+  </si>
+  <si>
+    <t>Bjørn</t>
   </si>
 </sst>
 </file>
@@ -510,7 +522,7 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -523,25 +535,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -616,7 +628,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
@@ -726,7 +738,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -737,7 +749,7 @@
         <v>19</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
@@ -747,7 +759,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -755,7 +767,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -763,7 +775,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -771,7 +783,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -779,7 +791,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -787,27 +799,39 @@
         <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>3</v>
       </c>
+      <c r="B29" s="2" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>4</v>
       </c>
+      <c r="B30" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>5</v>
       </c>
+      <c r="B31" s="2" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>6</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>